<commit_message>
completed first 9 exercises of part 9
</commit_message>
<xml_diff>
--- a/Study Plan for Java Prog 2.xlsx
+++ b/Study Plan for Java Prog 2.xlsx
@@ -188,22 +188,22 @@
     <t xml:space="preserve">Task 11</t>
   </si>
   <si>
+    <t xml:space="preserve">Task 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milestone 2 – Part 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milestone 2 – Part 9</t>
   </si>
   <si>
     <t xml:space="preserve">Milestone 3 – Part 10</t>
@@ -769,10 +769,10 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
@@ -814,15 +814,15 @@
       </c>
       <c r="D2" s="6" t="n">
         <f aca="false">SUM(FIN_ESTIMATES)</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">SUM(DAYS_LEFT)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F2" s="7" t="n">
         <f aca="false">COUNTIF(STATUSES,"Done")/(COUNTIF(STATUSES,"Not Started")+COUNTIF(STATUSES,"In Progress")+COUNTIF(STATUSES,"Done"))</f>
-        <v>0.103092783505155</v>
+        <v>0.185567010309278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,15 +884,15 @@
       </c>
       <c r="D5" s="19" t="n">
         <f aca="false">SUM(D2:D3)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E5" s="20" t="n">
         <f aca="false">SUM(E2:E3)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F5" s="21" t="n">
         <f aca="false">(D5-E5)/D5</f>
-        <v>0.32258064516129</v>
+        <v>0.527777777777778</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -906,15 +906,15 @@
       </c>
       <c r="D6" s="25" t="n">
         <f aca="false">SUM(D2:D4)</f>
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E6" s="26" t="n">
         <f aca="false">SUM(E2:E4)</f>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F6" s="27" t="n">
         <f aca="false">(D6-E6)/D6</f>
-        <v>0.232558139534884</v>
+        <v>0.395833333333333</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -950,19 +950,19 @@
         <v>44732</v>
       </c>
       <c r="B10" s="32" t="n">
-        <v>44764</v>
+        <v>44771</v>
       </c>
       <c r="C10" s="33" t="n">
         <f aca="true">MAX(0,(B10-TODAY()+1)/7*5)</f>
-        <v>17.8571428571429</v>
+        <v>17.1428571428571</v>
       </c>
       <c r="D10" s="34" t="n">
         <f aca="true">MAX(0,(B10-NOW()+1)/7*2)</f>
-        <v>6.88855476851833</v>
+        <v>6.58188304563477</v>
       </c>
       <c r="E10" s="34" t="n">
         <f aca="false">SUM(C10:D10)</f>
-        <v>24.7456976256612</v>
+        <v>23.7247401884919</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -991,15 +991,15 @@
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="35" t="str">
         <f aca="false">ROUND(TOTAL_INITIAL_ESTIMATE/(DEADLINE-STARTDATE+1),1) &amp; " h/day"</f>
-        <v>3.5 h/day</v>
+        <v>2.9 h/day</v>
       </c>
       <c r="B14" s="36" t="str">
         <f aca="false">ROUND(TOTAL_PLUS_EXTRA_TIME_SPENT/(DEADLINE-STARTDATE+1),1) &amp; " h/day"</f>
-        <v>1.3 h/day</v>
+        <v>1.2 h/day</v>
       </c>
       <c r="C14" s="36" t="str">
         <f aca="false">IF(TOTAL_DAYS_LEFT = 0, "N/A", ROUND(TOTAL_EXTRA_WORK_HOURS_LEFT/TOTAL_DAYS_LEFT,1) &amp; " h/day")</f>
-        <v>1.3 h/day</v>
+        <v>1.2 h/day</v>
       </c>
       <c r="D14" s="36" t="str">
         <f aca="true">IF(TODAY()&gt;DEADLINE, "N/A", ROUND((TOTAL_PLUS_EXTRA_TIME_SPENT-TOTAL_EXTRA_WORK_HOURS_LEFT)/(TODAY()-STARTDATE+1),1) &amp; " h/day")</f>
@@ -1061,10 +1061,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -1393,58 +1393,73 @@
       <c r="B14" s="41" t="n">
         <v>1</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E14" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="41" t="n">
         <v>1</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E15" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="41" t="n">
         <v>1</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E16" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="41" t="n">
         <v>1</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E17" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="41" t="n">
         <v>1</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E18" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -1465,10 +1480,10 @@
       </c>
       <c r="D21" s="10" t="n">
         <f aca="false">IF(E21 = "Done",0,C21)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1483,10 +1498,10 @@
       </c>
       <c r="D22" s="10" t="n">
         <f aca="false">IF(E22 = "Done",0,C22)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,14 +1512,14 @@
         <v>1</v>
       </c>
       <c r="C23" s="41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" s="10" t="n">
         <f aca="false">IF(E23 = "Done",0,C23)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,15 +1529,13 @@
       <c r="B24" s="41" t="n">
         <v>1</v>
       </c>
-      <c r="C24" s="41" t="n">
-        <v>1</v>
-      </c>
+      <c r="C24" s="41"/>
       <c r="D24" s="10" t="n">
         <f aca="false">IF(E24 = "Done",0,C24)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1548,7 @@
       <c r="C25" s="41"/>
       <c r="D25" s="10"/>
       <c r="E25" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1561,7 @@
       <c r="C26" s="41"/>
       <c r="D26" s="10"/>
       <c r="E26" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,7 +1574,7 @@
       <c r="C27" s="41"/>
       <c r="D27" s="10"/>
       <c r="E27" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,7 +1587,7 @@
       <c r="C28" s="41"/>
       <c r="D28" s="10"/>
       <c r="E28" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1587,7 +1600,7 @@
       <c r="C29" s="41"/>
       <c r="D29" s="10"/>
       <c r="E29" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,7 +1613,7 @@
       <c r="C30" s="41"/>
       <c r="D30" s="10"/>
       <c r="E30" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,12 +1626,12 @@
       <c r="C31" s="41"/>
       <c r="D31" s="10"/>
       <c r="E31" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" s="41" t="n">
         <v>1</v>
@@ -1626,7 +1639,7 @@
       <c r="C32" s="41"/>
       <c r="D32" s="10"/>
       <c r="E32" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,7 +1699,7 @@
       <c r="C37" s="41"/>
       <c r="D37" s="10"/>
       <c r="E37" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,7 +1712,7 @@
       <c r="C38" s="41"/>
       <c r="D38" s="10"/>
       <c r="E38" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1712,7 +1725,7 @@
       <c r="C39" s="41"/>
       <c r="D39" s="10"/>
       <c r="E39" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1725,7 +1738,7 @@
       <c r="C40" s="41"/>
       <c r="D40" s="10"/>
       <c r="E40" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1751,7 @@
       <c r="C41" s="41"/>
       <c r="D41" s="10"/>
       <c r="E41" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,7 +1764,7 @@
       <c r="C42" s="41"/>
       <c r="D42" s="10"/>
       <c r="E42" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,73 +1797,73 @@
         <v>1</v>
       </c>
       <c r="E45" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E46" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E48" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E49" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1877,7 +1890,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +1921,7 @@
       <c r="C56" s="41"/>
       <c r="D56" s="10"/>
       <c r="E56" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1921,7 +1934,7 @@
       <c r="C57" s="41"/>
       <c r="D57" s="10"/>
       <c r="E57" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1947,7 @@
       <c r="C58" s="41"/>
       <c r="D58" s="10"/>
       <c r="E58" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1947,7 +1960,7 @@
       <c r="C59" s="41"/>
       <c r="D59" s="10"/>
       <c r="E59" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1973,7 @@
       <c r="C60" s="41"/>
       <c r="D60" s="10"/>
       <c r="E60" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,7 +1986,7 @@
       <c r="C61" s="41"/>
       <c r="D61" s="10"/>
       <c r="E61" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1984,7 +1997,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,29 +2019,29 @@
         <v>1</v>
       </c>
       <c r="E64" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B65" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E66" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="E69" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,7 +2086,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,7 +2099,7 @@
       <c r="C71" s="41"/>
       <c r="D71" s="10"/>
       <c r="E71" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2099,7 +2112,7 @@
       <c r="C72" s="41"/>
       <c r="D72" s="10"/>
       <c r="E72" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,7 +2125,7 @@
       <c r="C73" s="41"/>
       <c r="D73" s="10"/>
       <c r="E73" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,7 +2138,7 @@
       <c r="C74" s="41"/>
       <c r="D74" s="10"/>
       <c r="E74" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,7 +2151,7 @@
       <c r="C75" s="41"/>
       <c r="D75" s="10"/>
       <c r="E75" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,7 +2164,7 @@
       <c r="C76" s="41"/>
       <c r="D76" s="10"/>
       <c r="E76" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2162,7 +2175,7 @@
         <v>1</v>
       </c>
       <c r="E77" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="E78" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,18 +2197,18 @@
         <v>1</v>
       </c>
       <c r="E79" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B80" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E80" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,7 +2235,7 @@
         <v>1</v>
       </c>
       <c r="E83" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="E84" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2266,7 @@
       <c r="C85" s="41"/>
       <c r="D85" s="10"/>
       <c r="E85" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,7 +2279,7 @@
       <c r="C86" s="41"/>
       <c r="D86" s="10"/>
       <c r="E86" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,7 +2292,7 @@
       <c r="C87" s="41"/>
       <c r="D87" s="10"/>
       <c r="E87" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,7 +2305,7 @@
       <c r="C88" s="41"/>
       <c r="D88" s="10"/>
       <c r="E88" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2318,7 @@
       <c r="C89" s="41"/>
       <c r="D89" s="10"/>
       <c r="E89" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,7 +2331,7 @@
       <c r="C90" s="41"/>
       <c r="D90" s="10"/>
       <c r="E90" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2342,7 @@
         <v>1</v>
       </c>
       <c r="E91" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="E92" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2351,29 +2364,29 @@
         <v>1</v>
       </c>
       <c r="E93" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B94" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E94" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B95" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E95" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2413,7 @@
         <v>1</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="E99" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,7 +2444,7 @@
       <c r="C100" s="41"/>
       <c r="D100" s="10"/>
       <c r="E100" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,7 +2457,7 @@
       <c r="C101" s="41"/>
       <c r="D101" s="10"/>
       <c r="E101" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2470,7 @@
       <c r="C102" s="41"/>
       <c r="D102" s="10"/>
       <c r="E102" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2470,7 +2483,7 @@
       <c r="C103" s="41"/>
       <c r="D103" s="10"/>
       <c r="E103" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2483,7 +2496,7 @@
       <c r="C104" s="41"/>
       <c r="D104" s="10"/>
       <c r="E104" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,7 +2509,7 @@
       <c r="C105" s="41"/>
       <c r="D105" s="10"/>
       <c r="E105" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,7 +2520,7 @@
         <v>1</v>
       </c>
       <c r="E106" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2531,7 @@
         <v>1</v>
       </c>
       <c r="E107" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2529,51 +2542,51 @@
         <v>1</v>
       </c>
       <c r="E108" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B109" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E109" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B110" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E110" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B111" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E111" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B112" s="41" t="n">
         <v>1</v>
       </c>
       <c r="E112" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2653,7 +2666,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -2703,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2721,7 +2734,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="42"/>
@@ -2759,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="42"/>
@@ -2797,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H7" s="43"/>
       <c r="I7" s="42"/>
@@ -2835,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="42"/>
@@ -2873,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="42"/>
@@ -2911,7 +2924,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H10" s="43"/>
       <c r="I10" s="42"/>
@@ -3061,7 +3074,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="4" min="4" style="0" width="15.13"/>
@@ -3111,7 +3124,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3129,7 +3142,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="42"/>
@@ -3167,7 +3180,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="42"/>
@@ -3205,7 +3218,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H7" s="43"/>
       <c r="I7" s="42"/>
@@ -3243,7 +3256,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="42"/>
@@ -3281,7 +3294,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="42"/>
@@ -3418,7 +3431,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="93.25"/>
   </cols>

</xml_diff>